<commit_message>
Add excel with concentrations
</commit_message>
<xml_diff>
--- a/Phantom/agar.xlsx
+++ b/Phantom/agar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mirth\Documents\BCIBAP\Phantom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D5FEE44-6F3E-48B5-952A-12C9477BD013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA88E07-FB3D-4609-9DED-8A23759B8038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{21A393F3-0AC4-4F0A-90A1-79255EA91CA1}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
   <si>
     <t>Agar</t>
   </si>
@@ -70,7 +70,133 @@
     <t>heat on 130, not boiling, 10 minutes 600 RPM</t>
   </si>
   <si>
-    <t>99g</t>
+    <t>2011.3 mg</t>
+  </si>
+  <si>
+    <t>3054.9 mg</t>
+  </si>
+  <si>
+    <t>3 g</t>
+  </si>
+  <si>
+    <t>2 g</t>
+  </si>
+  <si>
+    <t>1 g</t>
+  </si>
+  <si>
+    <t>99 g</t>
+  </si>
+  <si>
+    <t>98 g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">heated on 200, </t>
+  </si>
+  <si>
+    <t>4014.3 mg</t>
+  </si>
+  <si>
+    <t>4 g</t>
+  </si>
+  <si>
+    <t>96 g</t>
+  </si>
+  <si>
+    <t>97 g</t>
+  </si>
+  <si>
+    <t>1037.1 mg</t>
+  </si>
+  <si>
+    <t>95 g</t>
+  </si>
+  <si>
+    <t>heated on 300,</t>
+  </si>
+  <si>
+    <t>6033.4 mg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 g </t>
+  </si>
+  <si>
+    <t>94 g</t>
+  </si>
+  <si>
+    <t>5048.3 mg</t>
+  </si>
+  <si>
+    <t>5 g</t>
+  </si>
+  <si>
+    <t>3055.0 mg</t>
+  </si>
+  <si>
+    <t>Salt</t>
+  </si>
+  <si>
+    <t>542.5 mg</t>
+  </si>
+  <si>
+    <t>3022.4 mg</t>
+  </si>
+  <si>
+    <t>768.5 mg</t>
+  </si>
+  <si>
+    <t>3036.5 mg</t>
+  </si>
+  <si>
+    <t>1026.0 mg</t>
+  </si>
+  <si>
+    <t>3035.4 mg</t>
+  </si>
+  <si>
+    <t>3034.3 mg</t>
+  </si>
+  <si>
+    <t>1279.7 mg</t>
+  </si>
+  <si>
+    <t>1509.5 mg</t>
+  </si>
+  <si>
+    <t>3031.8 mg</t>
+  </si>
+  <si>
+    <t>1768.5 mg</t>
+  </si>
+  <si>
+    <t>(g)</t>
+  </si>
+  <si>
+    <t>Agar wt</t>
+  </si>
+  <si>
+    <t>DI wt</t>
+  </si>
+  <si>
+    <t>NaCl wt</t>
+  </si>
+  <si>
+    <t>Agar (mg)</t>
+  </si>
+  <si>
+    <t>Agar (g)</t>
+  </si>
+  <si>
+    <t>DI (mg)</t>
+  </si>
+  <si>
+    <t>NaCl (mg)</t>
+  </si>
+  <si>
+    <t>Tot (mg)</t>
+  </si>
+  <si>
+    <t>NaCl (g)</t>
   </si>
 </sst>
 </file>
@@ -422,18 +548,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F125A5FF-3239-46D6-A717-1BF123E36902}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="73.88671875" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,7 +568,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -455,7 +582,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -469,18 +596,752 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>97</v>
+      </c>
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>97</v>
+      </c>
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>97</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>96</v>
+      </c>
+      <c r="D18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>96</v>
+      </c>
+      <c r="D19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>96</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" t="s">
+        <v>52</v>
+      </c>
+      <c r="G21" t="s">
+        <v>45</v>
+      </c>
+      <c r="H21" t="s">
+        <v>46</v>
+      </c>
+      <c r="I21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>3055</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>97000</v>
+      </c>
+      <c r="D22">
+        <v>542.5</v>
+      </c>
+      <c r="E22">
+        <v>0.5</v>
+      </c>
+      <c r="F22">
+        <f xml:space="preserve"> A22 + C22 + D22</f>
+        <v>100597.5</v>
+      </c>
+      <c r="G22">
+        <f xml:space="preserve"> A22/F22</f>
+        <v>3.0368547926141305E-2</v>
+      </c>
+      <c r="H22">
+        <f>C22/F22</f>
+        <v>0.9642386739233082</v>
+      </c>
+      <c r="I22">
+        <f>D22/F22</f>
+        <v>5.392778150550461E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>3022.4</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>97000</v>
+      </c>
+      <c r="D23">
+        <v>768.5</v>
+      </c>
+      <c r="E23">
+        <v>0.75</v>
+      </c>
+      <c r="F23">
+        <f t="shared" ref="F23:F27" si="0" xml:space="preserve"> A23 + C23 + D23</f>
+        <v>100790.9</v>
+      </c>
+      <c r="G23">
+        <f t="shared" ref="G23:G27" si="1" xml:space="preserve"> A23/F23</f>
+        <v>2.9986834128874731E-2</v>
+      </c>
+      <c r="H23">
+        <f t="shared" ref="H23:H27" si="2">C23/F23</f>
+        <v>0.96238846959398128</v>
+      </c>
+      <c r="I23">
+        <f t="shared" ref="I23:I27" si="3">D23/F23</f>
+        <v>7.6246962771440684E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>3036.5</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <v>97000</v>
+      </c>
+      <c r="D24">
+        <v>1026</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>101062.5</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>3.0045763760049474E-2</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="2"/>
+        <v>0.95980210265924548</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="3"/>
+        <v>1.0152133580705009E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>3035.4</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>96000</v>
+      </c>
+      <c r="D25">
+        <v>1509.5</v>
+      </c>
+      <c r="E25">
+        <v>1.5</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>100544.9</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>3.0189497428512041E-2</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="2"/>
+        <v>0.95479730946074848</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="3"/>
+        <v>1.5013193110739582E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>3034.3</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>96000</v>
+      </c>
+      <c r="D26">
+        <v>1279.7</v>
+      </c>
+      <c r="E26">
+        <v>1.25</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>100314</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>3.0248021213389958E-2</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="2"/>
+        <v>0.95699503558825294</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="3"/>
+        <v>1.2756943198357159E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>3031.8</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>96000</v>
+      </c>
+      <c r="D27">
+        <v>1768.5</v>
+      </c>
+      <c r="E27">
+        <v>1.75</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>100800.3</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>3.0077291436632628E-2</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="2"/>
+        <v>0.95237811792226801</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="3"/>
+        <v>1.7544590641099284E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" t="s">
+        <v>52</v>
+      </c>
+      <c r="G28" t="s">
+        <v>45</v>
+      </c>
+      <c r="H28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>2011.3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29">
+        <v>98000</v>
+      </c>
+      <c r="F29">
+        <f xml:space="preserve"> A29 + C29</f>
+        <v>100011.3</v>
+      </c>
+      <c r="G29">
+        <f xml:space="preserve"> A29/F29</f>
+        <v>2.0110727487793877E-2</v>
+      </c>
+      <c r="H29">
+        <f>C29/F29</f>
+        <v>0.97988927251220614</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>3054.9</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30">
+        <v>97000</v>
+      </c>
+      <c r="F30">
+        <f t="shared" ref="F30:F41" si="4" xml:space="preserve"> A30 + C30</f>
+        <v>100054.9</v>
+      </c>
+      <c r="G30">
+        <f t="shared" ref="G30:G41" si="5" xml:space="preserve"> A30/F30</f>
+        <v>3.053223780144701E-2</v>
+      </c>
+      <c r="H30">
+        <f t="shared" ref="H30:H41" si="6">C30/F30</f>
+        <v>0.96946776219855302</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>4014.3</v>
+      </c>
+      <c r="B31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31">
+        <v>96000</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="4"/>
+        <v>100014.3</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="5"/>
+        <v>4.0137260371766841E-2</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="6"/>
+        <v>0.9598627396282331</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>1037.0999999999999</v>
+      </c>
+      <c r="B32" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32">
+        <v>99000</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="4"/>
+        <v>100037.1</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="5"/>
+        <v>1.0367153785945413E-2</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="6"/>
+        <v>0.98963284621405456</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>6033.4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33">
+        <v>94000</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="4"/>
+        <v>100033.4</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="5"/>
+        <v>6.0313855172372428E-2</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="6"/>
+        <v>0.93968614482762758</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>5048.3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34">
+        <v>95000</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="4"/>
+        <v>100048.3</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="5"/>
+        <v>5.045862848244298E-2</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="6"/>
+        <v>0.94954137151755702</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" t="s">
+        <v>50</v>
+      </c>
+      <c r="F35" t="s">
+        <v>52</v>
+      </c>
+      <c r="G35" t="s">
+        <v>45</v>
+      </c>
+      <c r="H35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>1009.4</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>99000</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="4"/>
+        <v>100009.4</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="5"/>
+        <v>1.0093051253182201E-2</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="6"/>
+        <v>0.98990694874681784</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>1406.1</v>
+      </c>
+      <c r="B37">
+        <v>1.4</v>
+      </c>
+      <c r="C37">
+        <v>99000</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="4"/>
+        <v>100406.1</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="5"/>
+        <v>1.4004129231192127E-2</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="6"/>
+        <v>0.98599587076880779</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>1798</v>
+      </c>
+      <c r="B38">
+        <v>1.8</v>
+      </c>
+      <c r="C38">
+        <v>98000</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="4"/>
+        <v>99798</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="5"/>
+        <v>1.8016393114090461E-2</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="6"/>
+        <v>0.98198360688590958</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>2205</v>
+      </c>
+      <c r="B39">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C39">
+        <v>98000</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="4"/>
+        <v>100205</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="5"/>
+        <v>2.2004889975550123E-2</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="6"/>
+        <v>0.97799511002444983</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>2590</v>
+      </c>
+      <c r="B40">
+        <v>2.6</v>
+      </c>
+      <c r="C40">
+        <v>97000</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="4"/>
+        <v>99590</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="5"/>
+        <v>2.6006627171402751E-2</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="6"/>
+        <v>0.97399337282859721</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>3000</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41">
+        <v>97000</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="4"/>
+        <v>100000</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="5"/>
+        <v>0.03</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="6"/>
+        <v>0.97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>